<commit_message>
A bunch of uncomitted changes waiting for a comit...
</commit_message>
<xml_diff>
--- a/output/01.technical_outliers_and_loq/fish_id_outliers.xlsx
+++ b/output/01.technical_outliers_and_loq/fish_id_outliers.xlsx
@@ -1193,19 +1193,19 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>1.94874654111428</v>
+        <v>0.148680460909429</v>
       </c>
       <c r="D15" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F15" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G15" t="n">
         <v>70.323325635104</v>
@@ -1220,19 +1220,19 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C16" t="n">
-        <v>0.148680460909429</v>
+        <v>1.94874654111428</v>
       </c>
       <c r="D16" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E16" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F16" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G16" t="n">
         <v>70.323325635104</v>
@@ -1301,19 +1301,19 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" t="n">
-        <v>1.86638865039454</v>
+        <v>0.235291712662006</v>
       </c>
       <c r="D19" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F19" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G19" t="n">
         <v>80.4653971403308</v>
@@ -1328,19 +1328,19 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.235291712662006</v>
+        <v>1.86638865039454</v>
       </c>
       <c r="D20" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E20" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F20" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G20" t="n">
         <v>80.4653971403308</v>
@@ -1409,19 +1409,19 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C23" t="n">
-        <v>2.56606890042473</v>
+        <v>0.156323737612081</v>
       </c>
       <c r="D23" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F23" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G23" t="n">
         <v>86.3241000936705</v>
@@ -1436,19 +1436,19 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>0.156323737612081</v>
+        <v>2.56606890042473</v>
       </c>
       <c r="D24" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E24" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F24" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G24" t="n">
         <v>86.3241000936705</v>
@@ -1517,19 +1517,19 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C27" t="n">
-        <v>2.11181141032987</v>
+        <v>0.266022755177212</v>
       </c>
       <c r="D27" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F27" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G27" t="n">
         <v>82.5809754281459</v>
@@ -1544,19 +1544,19 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C28" t="n">
-        <v>0.266022755177212</v>
+        <v>2.11181141032987</v>
       </c>
       <c r="D28" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E28" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F28" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G28" t="n">
         <v>82.5809754281459</v>
@@ -1679,19 +1679,19 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C33" t="n">
-        <v>1.67050217802252</v>
+        <v>0.30019725486973</v>
       </c>
       <c r="D33" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F33" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G33" t="n">
         <v>82.4687377881985</v>
@@ -1706,19 +1706,19 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C34" t="n">
-        <v>0.30019725486973</v>
+        <v>1.67050217802252</v>
       </c>
       <c r="D34" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E34" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F34" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G34" t="n">
         <v>82.4687377881985</v>
@@ -1841,19 +1841,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C39" t="n">
-        <v>1.5294305566648</v>
+        <v>0.24039613449405</v>
       </c>
       <c r="D39" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E39" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F39" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G39" t="n">
         <v>81.7801085254379</v>
@@ -1868,19 +1868,19 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C40" t="n">
-        <v>0.24039613449405</v>
+        <v>1.5294305566648</v>
       </c>
       <c r="D40" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E40" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F40" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G40" t="n">
         <v>81.7801085254379</v>
@@ -1976,19 +1976,19 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C44" t="n">
-        <v>2.53392624396228</v>
+        <v>0.282718699685655</v>
       </c>
       <c r="D44" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F44" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G44" t="n">
         <v>84.6122914013806</v>
@@ -2003,19 +2003,19 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C45" t="n">
-        <v>0.282718699685655</v>
+        <v>2.53392624396228</v>
       </c>
       <c r="D45" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E45" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F45" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G45" t="n">
         <v>84.6122914013806</v>
@@ -5486,19 +5486,19 @@
         <v>90</v>
       </c>
       <c r="B174" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C174" t="n">
-        <v>368.954287781932</v>
+        <v>5.60447071121296</v>
       </c>
       <c r="D174" t="n">
-        <v>79.272744650811</v>
+        <v>2.93832418726495</v>
       </c>
       <c r="E174" t="n">
-        <v>13.8326977284032</v>
+        <v>0.505013069090625</v>
       </c>
       <c r="F174" t="n">
-        <v>368.954287781932</v>
+        <v>82.9367697861274</v>
       </c>
       <c r="G174" t="n">
         <v>75.9294068504595</v>
@@ -5513,19 +5513,19 @@
         <v>90</v>
       </c>
       <c r="B175" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C175" t="n">
-        <v>5.60447071121296</v>
+        <v>11.1586861255176</v>
       </c>
       <c r="D175" t="n">
-        <v>2.93832418726495</v>
+        <v>4.45532071226407</v>
       </c>
       <c r="E175" t="n">
-        <v>0.505013069090625</v>
+        <v>0.612445844820796</v>
       </c>
       <c r="F175" t="n">
-        <v>82.9367697861274</v>
+        <v>29.8980160943351</v>
       </c>
       <c r="G175" t="n">
         <v>75.9294068504595</v>
@@ -5540,19 +5540,19 @@
         <v>90</v>
       </c>
       <c r="B176" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C176" t="n">
-        <v>11.1586861255176</v>
+        <v>368.954287781932</v>
       </c>
       <c r="D176" t="n">
-        <v>4.45532071226407</v>
+        <v>79.272744650811</v>
       </c>
       <c r="E176" t="n">
-        <v>0.612445844820796</v>
+        <v>13.8326977284032</v>
       </c>
       <c r="F176" t="n">
-        <v>29.8980160943351</v>
+        <v>368.954287781932</v>
       </c>
       <c r="G176" t="n">
         <v>75.9294068504595</v>
@@ -6516,19 +6516,19 @@
         <v>119</v>
       </c>
       <c r="B212" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C212" t="n">
-        <v>195.241531369012</v>
+        <v>8.7773100821808</v>
       </c>
       <c r="D212" t="n">
-        <v>79.272744650811</v>
+        <v>2.93832418726495</v>
       </c>
       <c r="E212" t="n">
-        <v>13.8326977284032</v>
+        <v>0.505013069090625</v>
       </c>
       <c r="F212" t="n">
-        <v>368.954287781932</v>
+        <v>82.9367697861274</v>
       </c>
       <c r="G212" t="n">
         <v>75.6524753282766</v>
@@ -6543,19 +6543,19 @@
         <v>119</v>
       </c>
       <c r="B213" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C213" t="n">
-        <v>8.7773100821808</v>
+        <v>12.6798957706955</v>
       </c>
       <c r="D213" t="n">
-        <v>2.93832418726495</v>
+        <v>4.45532071226407</v>
       </c>
       <c r="E213" t="n">
-        <v>0.505013069090625</v>
+        <v>0.612445844820796</v>
       </c>
       <c r="F213" t="n">
-        <v>82.9367697861274</v>
+        <v>29.8980160943351</v>
       </c>
       <c r="G213" t="n">
         <v>75.6524753282766</v>
@@ -6570,19 +6570,19 @@
         <v>119</v>
       </c>
       <c r="B214" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C214" t="n">
-        <v>12.6798957706955</v>
+        <v>195.241531369012</v>
       </c>
       <c r="D214" t="n">
-        <v>4.45532071226407</v>
+        <v>79.272744650811</v>
       </c>
       <c r="E214" t="n">
-        <v>0.612445844820796</v>
+        <v>13.8326977284032</v>
       </c>
       <c r="F214" t="n">
-        <v>29.8980160943351</v>
+        <v>368.954287781932</v>
       </c>
       <c r="G214" t="n">
         <v>75.6524753282766</v>
@@ -6597,19 +6597,19 @@
         <v>120</v>
       </c>
       <c r="B215" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C215" t="n">
-        <v>163.087533371086</v>
+        <v>12.2320200631017</v>
       </c>
       <c r="D215" t="n">
-        <v>79.272744650811</v>
+        <v>2.93832418726495</v>
       </c>
       <c r="E215" t="n">
-        <v>13.8326977284032</v>
+        <v>0.505013069090625</v>
       </c>
       <c r="F215" t="n">
-        <v>368.954287781932</v>
+        <v>82.9367697861274</v>
       </c>
       <c r="G215" t="n">
         <v>75.937998935604</v>
@@ -6624,19 +6624,19 @@
         <v>120</v>
       </c>
       <c r="B216" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C216" t="n">
-        <v>12.2320200631017</v>
+        <v>17.8060027505865</v>
       </c>
       <c r="D216" t="n">
-        <v>2.93832418726495</v>
+        <v>4.45532071226407</v>
       </c>
       <c r="E216" t="n">
-        <v>0.505013069090625</v>
+        <v>0.612445844820796</v>
       </c>
       <c r="F216" t="n">
-        <v>82.9367697861274</v>
+        <v>29.8980160943351</v>
       </c>
       <c r="G216" t="n">
         <v>75.937998935604</v>
@@ -6651,19 +6651,19 @@
         <v>120</v>
       </c>
       <c r="B217" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C217" t="n">
-        <v>17.8060027505865</v>
+        <v>163.087533371086</v>
       </c>
       <c r="D217" t="n">
-        <v>4.45532071226407</v>
+        <v>79.272744650811</v>
       </c>
       <c r="E217" t="n">
-        <v>0.612445844820796</v>
+        <v>13.8326977284032</v>
       </c>
       <c r="F217" t="n">
-        <v>29.8980160943351</v>
+        <v>368.954287781932</v>
       </c>
       <c r="G217" t="n">
         <v>75.937998935604</v>
@@ -6732,19 +6732,19 @@
         <v>121</v>
       </c>
       <c r="B220" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C220" t="n">
-        <v>199.237530662306</v>
+        <v>9.44194603434178</v>
       </c>
       <c r="D220" t="n">
-        <v>79.272744650811</v>
+        <v>2.93832418726495</v>
       </c>
       <c r="E220" t="n">
-        <v>13.8326977284032</v>
+        <v>0.505013069090625</v>
       </c>
       <c r="F220" t="n">
-        <v>368.954287781932</v>
+        <v>82.9367697861274</v>
       </c>
       <c r="G220" t="n">
         <v>78.2570310366797</v>
@@ -6759,19 +6759,19 @@
         <v>121</v>
       </c>
       <c r="B221" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C221" t="n">
-        <v>9.44194603434178</v>
+        <v>9.46034341782502</v>
       </c>
       <c r="D221" t="n">
-        <v>2.93832418726495</v>
+        <v>4.45532071226407</v>
       </c>
       <c r="E221" t="n">
-        <v>0.505013069090625</v>
+        <v>0.612445844820796</v>
       </c>
       <c r="F221" t="n">
-        <v>82.9367697861274</v>
+        <v>29.8980160943351</v>
       </c>
       <c r="G221" t="n">
         <v>78.2570310366797</v>
@@ -6786,19 +6786,19 @@
         <v>121</v>
       </c>
       <c r="B222" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C222" t="n">
-        <v>9.46034341782502</v>
+        <v>199.237530662306</v>
       </c>
       <c r="D222" t="n">
-        <v>4.45532071226407</v>
+        <v>79.272744650811</v>
       </c>
       <c r="E222" t="n">
-        <v>0.612445844820796</v>
+        <v>13.8326977284032</v>
       </c>
       <c r="F222" t="n">
-        <v>29.8980160943351</v>
+        <v>368.954287781932</v>
       </c>
       <c r="G222" t="n">
         <v>78.2570310366797</v>
@@ -7245,19 +7245,19 @@
         <v>133</v>
       </c>
       <c r="B239" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C239" t="n">
-        <v>2.10883831599954</v>
+        <v>0.174425298384311</v>
       </c>
       <c r="D239" t="n">
-        <v>0.675619363236724</v>
+        <v>0.0946495589522645</v>
       </c>
       <c r="E239" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.0223495702005731</v>
       </c>
       <c r="F239" t="n">
-        <v>8.07492237590225</v>
+        <v>0.48519837857757</v>
       </c>
       <c r="G239" t="n">
         <v>75.5517826825127</v>
@@ -7272,19 +7272,19 @@
         <v>133</v>
       </c>
       <c r="B240" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C240" t="n">
-        <v>0.174425298384311</v>
+        <v>2.10883831599954</v>
       </c>
       <c r="D240" t="n">
-        <v>0.0946495589522645</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E240" t="n">
-        <v>0.0223495702005731</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F240" t="n">
-        <v>0.48519837857757</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G240" t="n">
         <v>75.5517826825127</v>
@@ -7326,19 +7326,19 @@
         <v>134</v>
       </c>
       <c r="B242" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="C242" t="n">
-        <v>185.264644432407</v>
+        <v>117.931207923857</v>
       </c>
       <c r="D242" t="n">
-        <v>79.272744650811</v>
+        <v>53.6194671067111</v>
       </c>
       <c r="E242" t="n">
-        <v>13.8326977284032</v>
+        <v>17.2797769119108</v>
       </c>
       <c r="F242" t="n">
-        <v>368.954287781932</v>
+        <v>161.07593729738</v>
       </c>
       <c r="G242" t="n">
         <v>76.1621233859398</v>
@@ -7353,19 +7353,19 @@
         <v>134</v>
       </c>
       <c r="B243" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="C243" t="n">
-        <v>117.931207923857</v>
+        <v>5.85970749825892</v>
       </c>
       <c r="D243" t="n">
-        <v>53.6194671067111</v>
+        <v>2.73299221888054</v>
       </c>
       <c r="E243" t="n">
-        <v>17.2797769119108</v>
+        <v>1.25943300020396</v>
       </c>
       <c r="F243" t="n">
-        <v>161.07593729738</v>
+        <v>5.85970749825892</v>
       </c>
       <c r="G243" t="n">
         <v>76.1621233859398</v>
@@ -7380,19 +7380,19 @@
         <v>134</v>
       </c>
       <c r="B244" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C244" t="n">
-        <v>5.85970749825892</v>
+        <v>185.264644432407</v>
       </c>
       <c r="D244" t="n">
-        <v>2.73299221888054</v>
+        <v>79.272744650811</v>
       </c>
       <c r="E244" t="n">
-        <v>1.25943300020396</v>
+        <v>13.8326977284032</v>
       </c>
       <c r="F244" t="n">
-        <v>5.85970749825892</v>
+        <v>368.954287781932</v>
       </c>
       <c r="G244" t="n">
         <v>76.1621233859398</v>
@@ -7899,19 +7899,19 @@
         <v>149</v>
       </c>
       <c r="B263" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="C263" t="n">
-        <v>190.167355778697</v>
+        <v>0.246111439259697</v>
       </c>
       <c r="D263" t="n">
-        <v>79.272744650811</v>
+        <v>0.0946495589522645</v>
       </c>
       <c r="E263" t="n">
-        <v>13.8326977284032</v>
+        <v>0.0223495702005731</v>
       </c>
       <c r="F263" t="n">
-        <v>368.954287781932</v>
+        <v>0.48519837857757</v>
       </c>
       <c r="G263" t="n">
         <v>76.6232324493846</v>
@@ -7926,19 +7926,19 @@
         <v>149</v>
       </c>
       <c r="B264" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="C264" t="n">
-        <v>0.246111439259697</v>
+        <v>190.167355778697</v>
       </c>
       <c r="D264" t="n">
-        <v>0.0946495589522645</v>
+        <v>79.272744650811</v>
       </c>
       <c r="E264" t="n">
-        <v>0.0223495702005731</v>
+        <v>13.8326977284032</v>
       </c>
       <c r="F264" t="n">
-        <v>0.48519837857757</v>
+        <v>368.954287781932</v>
       </c>
       <c r="G264" t="n">
         <v>76.6232324493846</v>
@@ -8142,19 +8142,19 @@
         <v>153</v>
       </c>
       <c r="B272" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C272" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="D272" t="n">
-        <v>0.675619363236724</v>
+        <v>0.053802992568572</v>
       </c>
       <c r="E272" t="n">
-        <v>0.0482610082961072</v>
+        <v>0.005</v>
       </c>
       <c r="F272" t="n">
-        <v>8.07492237590225</v>
+        <v>0.488527763216259</v>
       </c>
       <c r="G272" t="n">
         <v>78.7320302765431</v>
@@ -8169,19 +8169,19 @@
         <v>153</v>
       </c>
       <c r="B273" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C273" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="D273" t="n">
-        <v>0.053802992568572</v>
+        <v>0.675619363236724</v>
       </c>
       <c r="E273" t="n">
-        <v>0.005</v>
+        <v>0.0482610082961072</v>
       </c>
       <c r="F273" t="n">
-        <v>0.488527763216259</v>
+        <v>8.07492237590225</v>
       </c>
       <c r="G273" t="n">
         <v>78.7320302765431</v>

</xml_diff>